<commit_message>
Updating main, removing functions from notebook, creating git ignore
</commit_message>
<xml_diff>
--- a/output/results.xlsx
+++ b/output/results.xlsx
@@ -28,27 +28,27 @@
     <t>text</t>
   </si>
   <si>
+    <t>FILE_1.pdf</t>
+  </si>
+  <si>
     <t>FILE_2.pdf</t>
   </si>
   <si>
+    <t>Multi_Estrategia-GER-2020_06.pdf</t>
+  </si>
+  <si>
+    <t>Multi_Estrategia-GER-2020_07.pdf</t>
+  </si>
+  <si>
+    <t>Multi_Estrategia-GER-2020_08.pdf</t>
+  </si>
+  <si>
     <t>Multi_Estrategia-GER-2020_09.pdf</t>
   </si>
   <si>
-    <t>FILE_1.pdf</t>
-  </si>
-  <si>
-    <t>Multi_Estrategia-GER-2020_08.pdf</t>
-  </si>
-  <si>
     <t>Multi_Estrategia-GER-2020_10.pdf</t>
   </si>
   <si>
-    <t>Multi_Estrategia-GER-2020_06.pdf</t>
-  </si>
-  <si>
-    <t>Multi_Estrategia-GER-2020_07.pdf</t>
-  </si>
-  <si>
     <t>regex</t>
   </si>
   <si>
@@ -61,21 +61,81 @@
     <t>[]</t>
   </si>
   <si>
+    <t>EAPC, com CNPJ de n° 87.376.109/0001-06, ins</t>
+  </si>
+  <si>
+    <t>['taxa de juros efetiva anual e a tá', 'taxa de mortalidade.  § 2º No cálc']</t>
+  </si>
+  <si>
+    <t>completo, CNPJ ou CPF.  Art. 11. As questões</t>
+  </si>
+  <si>
+    <t>, CNPJ ou CPF.  Art. 11. As questões judici</t>
+  </si>
+  <si>
+    <t>['taxa de juros efetiva anual e da t']</t>
+  </si>
+  <si>
+    <t>['taxa de mortalidade;  33. TAXA DE ']</t>
+  </si>
+  <si>
+    <t>minação e CNPJ; b) Identificação do plano: s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minação e CNPJ do(s) FIE(s) vinculado(s) ao </t>
+  </si>
+  <si>
+    <t>['taxa de administração do(s) FIE(s)', 'taxa de performance, quando aplicá', 'taxa de administração e taxa de pe', 'taxa poderá ser consultada no regu']</t>
+  </si>
+  <si>
+    <t>minação e CNPJ do(s) respectivo(s) FIE(s); I</t>
+  </si>
+  <si>
+    <t>['taxas de administração e performan', 'taxa de inscrição nem quaisquer ou', 'taxas, comissões ou valores, a qua']</t>
+  </si>
+  <si>
+    <t>['taxa de juros e na versão da tábua', 'taxa de administração e a taxa de ', 'taxas poderão ser consultadas no r']</t>
+  </si>
+  <si>
+    <t>minação e CNPJ do FIE no qual estarão aplica</t>
+  </si>
+  <si>
+    <t>minação e CNPJ do respectivo FIE;  VI - Demo</t>
+  </si>
+  <si>
+    <t>eração de CNPJ e, consequentemente, de denom</t>
+  </si>
+  <si>
+    <t>eração de CNPJ e denominação, quando for pre</t>
+  </si>
+  <si>
+    <t>['taxa máxima de administração e des', 'taxa máxima de administração e des']</t>
+  </si>
+  <si>
+    <t>['taxa de administração efetivamente']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Físicas - CPF; IV - Dados bancários para a </t>
+  </si>
+  <si>
+    <t>cimento e CPF do beneficiário (ou beneficiá</t>
+  </si>
+  <si>
+    <t>strado no CNPJ sob n.º 37.253.900/0001-50 se</t>
+  </si>
+  <si>
+    <t>['taxa de juros efetiva anual: 0,00 ']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nação e o CNPJ do novo FIE, no qual estarão </t>
+  </si>
+  <si>
+    <t>['taxa de rentabilidade do respectiv']</t>
+  </si>
+  <si>
     <t>EAPC, com CNPJ de n° 42.283.770/0001-39, ins</t>
   </si>
   <si>
-    <t>['taxa de juros efetiva anual e a tá', 'taxa de mortalidade.  § 2º No cálc']</t>
-  </si>
-  <si>
-    <t>completo, CNPJ ou CPF.  Art. 11. As questões</t>
-  </si>
-  <si>
-    <t>, CNPJ ou CPF.  Art. 11. As questões judici</t>
-  </si>
-  <si>
-    <t>['taxa de juros efetiva anual e da t']</t>
-  </si>
-  <si>
     <t xml:space="preserve">minação e CNPJ; b)  identificação do plano: </t>
   </si>
   <si>
@@ -85,9 +145,6 @@
     <t>['taxa de administração e da taxa de', 'taxa de administração e a taxa de ']</t>
   </si>
   <si>
-    <t xml:space="preserve">minação e CNPJ do(s) FIE(s) vinculado(s) ao </t>
-  </si>
-  <si>
     <t>['taxa de inscrição nem quaisquer ou', 'taxas, comissões ou valores, a qua']</t>
   </si>
   <si>
@@ -100,18 +157,12 @@
     <t>['taxa de juros e na versão da tábua', 'taxa de administração e a taxa de ', 'taxa de juros contratada e versão ']</t>
   </si>
   <si>
-    <t>minação e CNPJ do FIE no qual estarão aplica</t>
-  </si>
-  <si>
     <t>minação e CNPJ do respectivo FIE;   VI - dem</t>
   </si>
   <si>
     <t>Físicas - CPF;  IV - dados bancários para a</t>
   </si>
   <si>
-    <t>cimento e CPF do beneficiário (ou beneficiá</t>
-  </si>
-  <si>
     <t>['taxa de juros efetiva anual: 0% a.']</t>
   </si>
   <si>
@@ -124,67 +175,16 @@
     <t>nação e o CNPJ do novo FIE no qual estarão a</t>
   </si>
   <si>
-    <t>['taxa de rentabilidade do respectiv']</t>
+    <t>inscritanoCNPJsobonº62.375.134/0001-44.9,710</t>
+  </si>
+  <si>
+    <t>['taxadeadministraçãomáximapagapeloF', 'taxadeadministraçãoacimaeastaxasde', 'taxasdeadministração,cotizaçãoepúb']</t>
   </si>
   <si>
     <t>inscritanoCNPJsobonº62.375.134/0001-44.9,71V</t>
   </si>
   <si>
     <t>['taxasdeadministração,cotizaçãoepúb', 'taxadeadministraçãomáximapagapeloF', 'taxadeadministraçãoacimaeastaxasde']</t>
-  </si>
-  <si>
-    <t>EAPC, com CNPJ de n° 87.376.109/0001-06, ins</t>
-  </si>
-  <si>
-    <t>['taxa de mortalidade;  33. TAXA DE ']</t>
-  </si>
-  <si>
-    <t>minação e CNPJ; b) Identificação do plano: s</t>
-  </si>
-  <si>
-    <t>['taxa de administração do(s) FIE(s)', 'taxa de performance, quando aplicá', 'taxa de administração e taxa de pe', 'taxa poderá ser consultada no regu']</t>
-  </si>
-  <si>
-    <t>minação e CNPJ do(s) respectivo(s) FIE(s); I</t>
-  </si>
-  <si>
-    <t>['taxas de administração e performan', 'taxa de inscrição nem quaisquer ou', 'taxas, comissões ou valores, a qua']</t>
-  </si>
-  <si>
-    <t>['taxa de juros e na versão da tábua', 'taxa de administração e a taxa de ', 'taxas poderão ser consultadas no r']</t>
-  </si>
-  <si>
-    <t>minação e CNPJ do respectivo FIE;  VI - Demo</t>
-  </si>
-  <si>
-    <t>eração de CNPJ e, consequentemente, de denom</t>
-  </si>
-  <si>
-    <t>eração de CNPJ e denominação, quando for pre</t>
-  </si>
-  <si>
-    <t>['taxa máxima de administração e des', 'taxa máxima de administração e des']</t>
-  </si>
-  <si>
-    <t>['taxa de administração efetivamente']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Físicas - CPF; IV - Dados bancários para a </t>
-  </si>
-  <si>
-    <t>strado no CNPJ sob n.º 37.253.900/0001-50 se</t>
-  </si>
-  <si>
-    <t>['taxa de juros efetiva anual: 0,00 ']</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nação e o CNPJ do novo FIE, no qual estarão </t>
-  </si>
-  <si>
-    <t>inscritanoCNPJsobonº62.375.134/0001-44.9,710</t>
-  </si>
-  <si>
-    <t>['taxadeadministraçãomáximapagapeloF', 'taxadeadministraçãoacimaeastaxasde', 'taxasdeadministração,cotizaçãoepúb']</t>
   </si>
   <si>
     <t>erformanceCNPJRetorno anualizadoData de iníc</t>
@@ -674,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -682,13 +682,13 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -696,13 +696,13 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -716,7 +716,7 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -730,7 +730,7 @@
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -738,13 +738,13 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -752,13 +752,13 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -772,7 +772,7 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -786,7 +786,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -800,7 +800,7 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -814,7 +814,7 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -842,7 +842,7 @@
         <v>12</v>
       </c>
       <c r="D21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -864,13 +864,13 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C23">
         <v>13</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -878,13 +878,13 @@
         <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -895,10 +895,10 @@
         <v>11</v>
       </c>
       <c r="C25">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -906,13 +906,13 @@
         <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C26">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -920,13 +920,13 @@
         <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D27" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -940,7 +940,7 @@
         <v>16</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -948,13 +948,13 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C29">
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -962,13 +962,13 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C30">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -976,13 +976,13 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -993,10 +993,10 @@
         <v>11</v>
       </c>
       <c r="C32">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1007,10 +1007,10 @@
         <v>11</v>
       </c>
       <c r="C33">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1018,13 +1018,13 @@
         <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D34" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1035,10 +1035,10 @@
         <v>11</v>
       </c>
       <c r="C35">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D35" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1049,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="C36">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
@@ -1060,13 +1060,13 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C37">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1077,10 +1077,10 @@
         <v>11</v>
       </c>
       <c r="C38">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1091,49 +1091,49 @@
         <v>11</v>
       </c>
       <c r="C39">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="D42" t="s">
         <v>14</v>
@@ -1141,279 +1141,279 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="D43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
         <v>11</v>
       </c>
       <c r="C44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" t="s">
         <v>12</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C47">
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B49" t="s">
         <v>11</v>
       </c>
       <c r="C49">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
       </c>
       <c r="C50">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D50" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52">
         <v>6</v>
       </c>
-      <c r="B52" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52">
-        <v>7</v>
-      </c>
       <c r="D52" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53">
         <v>6</v>
       </c>
-      <c r="B53" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53">
-        <v>7</v>
-      </c>
       <c r="D53" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C54">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C55">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B56" t="s">
         <v>12</v>
       </c>
       <c r="C56">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D56" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B57" t="s">
         <v>11</v>
       </c>
       <c r="C57">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D57" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C58">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D58" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C59">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D59" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
         <v>11</v>
       </c>
       <c r="C60">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D60" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
       </c>
       <c r="C61">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>46</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
         <v>11</v>
       </c>
       <c r="C62">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D62" t="s">
         <v>14</v>
@@ -1421,13 +1421,13 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B63" t="s">
         <v>12</v>
       </c>
       <c r="C63">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D63" t="s">
         <v>47</v>
@@ -1435,21 +1435,21 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C64">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D64" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B65" t="s">
         <v>11</v>
@@ -1458,12 +1458,12 @@
         <v>13</v>
       </c>
       <c r="D65" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
@@ -1472,12 +1472,12 @@
         <v>14</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B67" t="s">
         <v>11</v>
@@ -1491,49 +1491,49 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B68" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C68">
         <v>16</v>
       </c>
       <c r="D68" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B69" t="s">
         <v>13</v>
       </c>
       <c r="C69">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D69" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C70">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D70" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B71" t="s">
         <v>11</v>
@@ -1547,7 +1547,7 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B72" t="s">
         <v>11</v>
@@ -1561,35 +1561,35 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B73" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C73">
         <v>19</v>
       </c>
       <c r="D73" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B74" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C74">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D74" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B75" t="s">
         <v>11</v>
@@ -1598,12 +1598,12 @@
         <v>20</v>
       </c>
       <c r="D75" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B76" t="s">
         <v>11</v>
@@ -1612,12 +1612,12 @@
         <v>21</v>
       </c>
       <c r="D76" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B77" t="s">
         <v>11</v>
@@ -1626,12 +1626,12 @@
         <v>22</v>
       </c>
       <c r="D77" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B78" t="s">
         <v>11</v>
@@ -1640,32 +1640,32 @@
         <v>23</v>
       </c>
       <c r="D78" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C79">
         <v>24</v>
       </c>
       <c r="D79" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B80" t="s">
         <v>11</v>
       </c>
       <c r="C80">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D80" t="s">
         <v>14</v>
@@ -1673,16 +1673,16 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C81">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D81" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -1690,13 +1690,13 @@
         <v>6</v>
       </c>
       <c r="B82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C82">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="D82" t="s">
-        <v>14</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -1707,10 +1707,10 @@
         <v>11</v>
       </c>
       <c r="C83">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -1752,7 +1752,7 @@
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -1760,27 +1760,27 @@
         <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C87">
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C88">
         <v>1</v>
       </c>
       <c r="D88" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -1788,27 +1788,27 @@
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C89">
         <v>1</v>
       </c>
       <c r="D89" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C90">
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -1822,7 +1822,7 @@
         <v>1</v>
       </c>
       <c r="D91" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -1836,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="D92" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>